<commit_message>
DONALD-4 updated algorithm for EDU_LEVEL, status_detail for food groups on P2 and DIET_ASSESS_INSTR to 3
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_DONALD_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_DONALD_P1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545390A8-E807-4E88-856D-14D50E6B0869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520605E8-3601-49FF-96D8-D6FFC3541D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -892,20 +892,21 @@
     <t>case_when</t>
   </si>
   <si>
+    <t>m_schulab;v_schulab;m_berufab;v_berufab;</t>
+  </si>
+  <si>
+    <t>Highest level of education [ISCED 2011]</t>
+  </si>
+  <si>
     <t>case_when(
   m_berufab == 5 | v_berufab == 5 ~ 7,
   m_berufab %in% c(3, 4) | v_berufab %in% c(3, 4) ~ 6,
-  m_berufab %in% c(1, 2) | v_berufab %in% c(1, 2) ~ 5,
+  m_berufab %in% c(1, 2) | v_berufab %in% c(1, 2) ~ 4,
   m_schulab %in% c(3, 4) | v_schulab %in% c(3, 4) ~ 3,
   m_schulab %in% c(1, 2) | v_schulab %in% c(1, 2) ~ 2,
+  m_schulab == 5 | v_schulab == 5 | m_berufab %in% c(6, 7, 8)| v_berufab %in% c(6, 7, 8) ~ 9,
   TRUE ~ NA_real_
-  )</t>
-  </si>
-  <si>
-    <t>m_schulab;v_schulab;m_berufab;v_berufab;</t>
-  </si>
-  <si>
-    <t>Highest level of education [ISCED 2011]</t>
+)</t>
   </si>
 </sst>
 </file>
@@ -1265,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1415,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="2" customFormat="1" ht="330" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1422,7 +1423,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>272</v>
@@ -1431,13 +1432,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>289</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>273</v>
@@ -5539,7 +5540,7 @@
         <v>288</v>
       </c>
       <c r="H129" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I129" s="6"/>
       <c r="J129" s="2" t="s">

</xml_diff>

<commit_message>
DONALD-5 Adjustments to reflect recoding of the smoking variable in both P1 and P2 and mock datasets
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_DONALD_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_DONALD_P1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520605E8-3601-49FF-96D8-D6FFC3541D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0970B2A-2293-4987-9F82-F85A236B415D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="295">
   <si>
     <t>index</t>
   </si>
@@ -907,6 +907,12 @@
   m_schulab == 5 | v_schulab == 5 | m_berufab %in% c(6, 7, 8)| v_berufab %in% c(6, 7, 8) ~ 9,
   TRUE ~ NA_real_
 )</t>
+  </si>
+  <si>
+    <t>recode</t>
+  </si>
+  <si>
+    <t>recode(1=3;0=1;)</t>
   </si>
 </sst>
 </file>
@@ -986,7 +992,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1267,10 +1273,10 @@
   <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G7" sqref="G7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="53.140625" customWidth="1"/>
@@ -1501,11 +1507,11 @@
       <c r="F7" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>269</v>
+      <c r="G7" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>279</v>

</xml_diff>